<commit_message>
Update import curriculum class with id auto increment
Related Work Items: #1521
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT UIS-ThoiKhoaBieu_TieuChuan - Copy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\Excel dữ liệu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99D64A7-2601-4384-881C-5F2DD4019431}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17EFE50E-D86C-4B34-99A7-E5836D4318CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5232" yWindow="984" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9666" uniqueCount="865">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9673" uniqueCount="865">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -5431,7 +5431,7 @@
     <t>Ghi Chú 1</t>
   </si>
   <si>
-    <t xml:space="preserve">197pm21905   </t>
+    <t>197pm21905</t>
   </si>
 </sst>
 </file>
@@ -6352,10 +6352,10 @@
   <dimension ref="A1:AF312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="M19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q2" sqref="Q2"/>
+      <selection pane="bottomRight" activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6523,9 +6523,7 @@
       <c r="O2" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="10" t="s">
-        <v>864</v>
-      </c>
+      <c r="P2" s="10"/>
       <c r="Q2" s="10" t="s">
         <v>43</v>
       </c>
@@ -8824,7 +8822,7 @@
         <v>112</v>
       </c>
       <c r="P26" s="11" t="s">
-        <v>38</v>
+        <v>864</v>
       </c>
       <c r="Q26" s="11" t="s">
         <v>140</v>

</xml_diff>